<commit_message>
Deal Chat Testcases Updated
</commit_message>
<xml_diff>
--- a/TestData/Chat.xlsx
+++ b/TestData/Chat.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="Chat Details" sheetId="2" r:id="rId3"/>
+    <sheet name="Deal_Chat Details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="69">
   <si>
     <t>Account Type</t>
   </si>
@@ -181,6 +182,48 @@
   </si>
   <si>
     <t>Karthikeyan</t>
+  </si>
+  <si>
+    <t>Automation Test ID</t>
+  </si>
+  <si>
+    <t>Deal Name</t>
+  </si>
+  <si>
+    <t>Deals_Chat_ShipperUser_TC001</t>
+  </si>
+  <si>
+    <t>AutoDeal</t>
+  </si>
+  <si>
+    <t>Send Message</t>
+  </si>
+  <si>
+    <t>Message send successfully</t>
+  </si>
+  <si>
+    <t>Hi John</t>
+  </si>
+  <si>
+    <t>Opertion</t>
+  </si>
+  <si>
+    <t>SEND</t>
+  </si>
+  <si>
+    <t>Message verified successfully</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>Deals_Chat_ShipperAdmin_TC002</t>
+  </si>
+  <si>
+    <t>Deals_Chat_CarrierUser_TC003</t>
+  </si>
+  <si>
+    <t>Hi Stan</t>
   </si>
 </sst>
 </file>
@@ -265,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -283,6 +326,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -590,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -673,7 +719,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,4 +1734,164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Location filter, Export deal, Negotiations and Chat Connection test cases updated
</commit_message>
<xml_diff>
--- a/TestData/Chat.xlsx
+++ b/TestData/Chat.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="Chat Details" sheetId="2" r:id="rId3"/>
     <sheet name="Deal_Chat Details" sheetId="4" r:id="rId4"/>
+    <sheet name="Deal_Chat_Connection" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="78">
   <si>
     <t>Account Type</t>
   </si>
@@ -224,6 +225,33 @@
   </si>
   <si>
     <t>Hi Stan</t>
+  </si>
+  <si>
+    <t>ChatConnection_TC001</t>
+  </si>
+  <si>
+    <t>No Channel Found</t>
+  </si>
+  <si>
+    <t>VERIFY_BANNER</t>
+  </si>
+  <si>
+    <t>Get Started Button is Disabled</t>
+  </si>
+  <si>
+    <t>ACCEPT_CONNECTION</t>
+  </si>
+  <si>
+    <t>Connection Accepted</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ChatConnection_TC002</t>
+  </si>
+  <si>
+    <t>Hi Zeb</t>
   </si>
 </sst>
 </file>
@@ -308,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -329,6 +357,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1740,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,10 +1797,10 @@
         <v>62</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>13</v>
@@ -1890,6 +1919,242 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>